<commit_message>
add more items in elimination list and to add list
</commit_message>
<xml_diff>
--- a/Hypothyroidism.xlsx
+++ b/Hypothyroidism.xlsx
@@ -1767,7 +1767,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1840,12 +1840,47 @@
         <v>18</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>2</v>
@@ -1854,33 +1889,68 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="H4" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s" s="0">
-        <v>26</v>
+      <c r="H5" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>2</v>
@@ -1889,33 +1959,68 @@
         <v>3</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>33</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s" s="0">
+        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>2</v>
@@ -1924,33 +2029,68 @@
         <v>3</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="J8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K8" t="s" s="0">
-        <v>40</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s" s="0">
+        <v>66</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>2</v>
@@ -1959,33 +2099,68 @@
         <v>3</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s" s="0">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="F11" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="H10" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="I10" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="J10" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K10" t="s" s="0">
-        <v>46</v>
+      <c r="G11" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s" s="0">
+        <v>79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>2</v>
@@ -1994,33 +2169,68 @@
         <v>3</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="J12" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>52</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K13" t="s" s="0">
+        <v>91</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>2</v>
@@ -2029,269 +2239,59 @@
         <v>3</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="F14" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="J14" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s" s="0">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="F15" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="G14" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="H14" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="I14" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="J14" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K14" t="s" s="0">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E16" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="F16" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="G16" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H16" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="I16" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="J16" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K16" t="s" s="0">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="F18" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="G18" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="H18" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="I18" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="J18" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K18" t="s" s="0">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
-        <v>74</v>
-      </c>
-      <c r="B20" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="C20" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E20" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="F20" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="G20" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="H20" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="I20" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="J20" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K20" t="s" s="0">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="B22" t="s" s="0">
-        <v>81</v>
-      </c>
-      <c r="C22" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E22" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="F22" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="G22" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="H22" t="s" s="0">
-        <v>83</v>
-      </c>
-      <c r="I22" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="J22" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K22" t="s" s="0">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="B24" t="s" s="0">
-        <v>87</v>
-      </c>
-      <c r="C24" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="F24" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G24" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H24" t="s" s="0">
-        <v>89</v>
-      </c>
-      <c r="I24" t="s" s="0">
-        <v>90</v>
-      </c>
-      <c r="J24" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K24" t="s" s="0">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="B26" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="C26" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E26" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="F26" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s" s="0">
+      <c r="G15" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="H26" t="s" s="0">
-        <v>96</v>
-      </c>
-      <c r="I26" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="J26" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K26" t="s" s="0">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="B28" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="C28" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E28" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="F28" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="G28" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="H28" t="s" s="0">
+      <c r="H15" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="I28" t="s" s="0">
+      <c r="I15" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="J28" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K28" t="s" s="0">
+      <c r="J15" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s" s="0">
         <v>104</v>
       </c>
     </row>

</xml_diff>